<commit_message>
resolve by type with depends
</commit_message>
<xml_diff>
--- a/Iocy.xlsx
+++ b/Iocy.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Iterations" sheetId="1" r:id="rId1"/>
+    <sheet name="Limitations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Resolve Method</t>
   </si>
@@ -50,13 +51,22 @@
   </si>
   <si>
     <t>TypedFactory Facility</t>
+  </si>
+  <si>
+    <t>Register with simple parameters</t>
+  </si>
+  <si>
+    <t>LifeStyle Singleton</t>
+  </si>
+  <si>
+    <t>Services with only one constructor supported</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +76,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,12 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,14 +460,22 @@
       <c r="B3" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -466,7 +493,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -475,13 +502,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
@@ -489,4 +521,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="54.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>